<commit_message>
fluxogramas, documentação e backlog
</commit_message>
<xml_diff>
--- a/sprint_grupo1/TI/Backlog_TecnoSolo ATUALIZADO.xlsx
+++ b/sprint_grupo1/TI/Backlog_TecnoSolo ATUALIZADO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\Pesquisa e inovação\sprint_01\sprint_grupo7\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\Pesquisa e inovação\sprint_01\sprint_grupo1\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44B706-0B97-49A2-95D5-6789E69B399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{556C227A-4542-4BFE-AE3A-0CCAF12498E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1824" yWindow="0" windowWidth="21216" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="107">
   <si>
     <t>Descrição</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Documento com planejaento para uma parada no sistema planejada ou não.</t>
   </si>
   <si>
-    <t>Diagrama do passo a passo do suporte na ferramenta de HelpDesk</t>
-  </si>
-  <si>
     <t>Ferramenta de helpDesk</t>
   </si>
   <si>
@@ -344,13 +341,22 @@
     <t>Integração API dashboard</t>
   </si>
   <si>
-    <t>Ferramenta de Help Desk FreshDesk para abrir tickets e chamados</t>
-  </si>
-  <si>
-    <t>Passo a passo para o cliente conseguir fazer instalação do sistema</t>
-  </si>
-  <si>
-    <t>Conexão com login e cadastro com banco de dados</t>
+    <t>Mostrar o analytics com os dados  coletados pelo sensor, sendo exibidos de forma dinamica</t>
+  </si>
+  <si>
+    <t>Graficos dinamicos atualizando sempre com os dados captados pelo sensor no banco de dados.</t>
+  </si>
+  <si>
+    <t>Diagrama do passo a passo do suporte na ferramenta de HelpDesk.</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk FreshDesk para abrir tickets e chamados.</t>
+  </si>
+  <si>
+    <t>Passo a passo para o cliente conseguir fazer instalação do sistema.</t>
+  </si>
+  <si>
+    <t>Conexão com login e cadastro com banco de dados.</t>
   </si>
 </sst>
 </file>
@@ -860,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1134,10 +1140,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1344,10 +1347,29 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1377,36 +1399,17 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1497,7 +1500,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:H39" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:H39" headerRowDxfId="12" dataDxfId="10" totalsRowDxfId="8" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A1:H39" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1824,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DM42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3615,7 +3618,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="82" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C34" s="83" t="s">
         <v>28</v>
@@ -3640,7 +3643,9 @@
       <c r="A35" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="84"/>
+      <c r="B35" s="84" t="s">
+        <v>101</v>
+      </c>
       <c r="C35" s="66" t="s">
         <v>28</v>
       </c>
@@ -3662,10 +3667,10 @@
     </row>
     <row r="36" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="87" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C36" s="87" t="s">
         <v>6</v>
@@ -3688,10 +3693,10 @@
     </row>
     <row r="37" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="89" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C37" s="89" t="s">
         <v>6</v>
@@ -3714,10 +3719,10 @@
     </row>
     <row r="38" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" s="89" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C38" s="89" t="s">
         <v>28</v>
@@ -3740,9 +3745,11 @@
     </row>
     <row r="39" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="87" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="91"/>
+        <v>100</v>
+      </c>
+      <c r="B39" s="91" t="s">
+        <v>102</v>
+      </c>
       <c r="C39" s="91" t="s">
         <v>28</v>
       </c>
@@ -3763,34 +3770,34 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="93"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="93"/>
-      <c r="H40" s="94"/>
+      <c r="A40" s="87"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="93"/>
     </row>
     <row r="41" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="93"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="94"/>
+      <c r="A41" s="87"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="93"/>
     </row>
     <row r="42" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="93"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="93"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="93"/>
-      <c r="H42" s="94"/>
+      <c r="A42" s="87"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>